<commit_message>
feat: more data extraction & skills key
</commit_message>
<xml_diff>
--- a/green_jobs.xlsx
+++ b/green_jobs.xlsx
@@ -25,7 +25,7 @@
     <t xml:space="preserve">SOC2010 Unit Group Titles</t>
   </si>
   <si>
-    <t xml:space="preserve">SOC2010 4-digitGreen Category</t>
+    <t xml:space="preserve">SOC2010 4-digit</t>
   </si>
   <si>
     <t xml:space="preserve">Green Category</t>
@@ -352,6 +352,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -436,12 +437,12 @@
   <dimension ref="A1:C101"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topLeft" activeCell="B26" activeCellId="0" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="57.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="57.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="56.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="52.79"/>
   </cols>

</xml_diff>